<commit_message>
updated order form for ny
</commit_message>
<xml_diff>
--- a/order_forms/order_ny_template_xlsx.xlsx
+++ b/order_forms/order_ny_template_xlsx.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akeln\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F6AB9A-40CF-4CC2-8D0F-852466F54CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ADF5338-F4C9-468F-9FF3-E21F14E244F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1345,142 +1345,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1497,6 +1362,72 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1505,6 +1436,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1512,29 +1452,98 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1542,6 +1551,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1553,24 +1571,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1883,201 +1883,201 @@
   <dimension ref="A1:AK43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AO19" sqref="AO19"/>
+      <selection activeCell="AJ14" sqref="AJ14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="1" max="1" width="3.68359375" customWidth="1"/>
     <col min="2" max="2" width="4" customWidth="1"/>
-    <col min="3" max="3" width="3.5703125" customWidth="1"/>
-    <col min="4" max="4" width="4.42578125" customWidth="1"/>
+    <col min="3" max="3" width="3.578125" customWidth="1"/>
+    <col min="4" max="4" width="4.41796875" customWidth="1"/>
     <col min="5" max="5" width="4" customWidth="1"/>
-    <col min="6" max="6" width="4.28515625" customWidth="1"/>
-    <col min="7" max="7" width="5.42578125" style="53" customWidth="1"/>
-    <col min="8" max="8" width="4.42578125" customWidth="1"/>
-    <col min="9" max="9" width="5.85546875" customWidth="1"/>
-    <col min="10" max="10" width="5.140625" customWidth="1"/>
-    <col min="11" max="11" width="3.5703125" customWidth="1"/>
-    <col min="12" max="12" width="5.28515625" customWidth="1"/>
-    <col min="13" max="13" width="3.5703125" customWidth="1"/>
-    <col min="14" max="14" width="5.140625" customWidth="1"/>
-    <col min="15" max="15" width="3.5703125" customWidth="1"/>
-    <col min="16" max="16" width="5.140625" customWidth="1"/>
-    <col min="17" max="17" width="7.42578125" customWidth="1"/>
-    <col min="18" max="18" width="5.140625" customWidth="1"/>
+    <col min="6" max="6" width="4.26171875" customWidth="1"/>
+    <col min="7" max="7" width="5.41796875" style="53" customWidth="1"/>
+    <col min="8" max="8" width="4.41796875" customWidth="1"/>
+    <col min="9" max="9" width="5.83984375" customWidth="1"/>
+    <col min="10" max="10" width="5.15625" customWidth="1"/>
+    <col min="11" max="11" width="3.578125" customWidth="1"/>
+    <col min="12" max="12" width="5.26171875" customWidth="1"/>
+    <col min="13" max="13" width="3.578125" customWidth="1"/>
+    <col min="14" max="14" width="5.15625" customWidth="1"/>
+    <col min="15" max="15" width="3.578125" customWidth="1"/>
+    <col min="16" max="16" width="5.15625" customWidth="1"/>
+    <col min="17" max="17" width="7.41796875" customWidth="1"/>
+    <col min="18" max="18" width="5.15625" customWidth="1"/>
     <col min="19" max="19" width="7" customWidth="1"/>
-    <col min="20" max="21" width="4.42578125" customWidth="1"/>
-    <col min="22" max="22" width="5.140625" customWidth="1"/>
-    <col min="23" max="23" width="3.42578125" customWidth="1"/>
-    <col min="24" max="24" width="5.85546875" customWidth="1"/>
-    <col min="25" max="25" width="3.5703125" customWidth="1"/>
-    <col min="26" max="26" width="5.5703125" customWidth="1"/>
-    <col min="27" max="27" width="3.7109375" customWidth="1"/>
+    <col min="20" max="21" width="4.41796875" customWidth="1"/>
+    <col min="22" max="22" width="5.15625" customWidth="1"/>
+    <col min="23" max="23" width="3.41796875" customWidth="1"/>
+    <col min="24" max="24" width="5.83984375" customWidth="1"/>
+    <col min="25" max="25" width="3.578125" customWidth="1"/>
+    <col min="26" max="26" width="5.578125" customWidth="1"/>
+    <col min="27" max="27" width="3.68359375" customWidth="1"/>
     <col min="28" max="28" width="6" customWidth="1"/>
-    <col min="29" max="29" width="6.140625" customWidth="1"/>
-    <col min="30" max="30" width="3.7109375" customWidth="1"/>
-    <col min="31" max="31" width="3.85546875" customWidth="1"/>
-    <col min="32" max="32" width="4.28515625" customWidth="1"/>
-    <col min="33" max="33" width="4.7109375" customWidth="1"/>
+    <col min="29" max="29" width="6.15625" customWidth="1"/>
+    <col min="30" max="30" width="3.68359375" customWidth="1"/>
+    <col min="31" max="31" width="3.83984375" customWidth="1"/>
+    <col min="32" max="32" width="4.26171875" customWidth="1"/>
+    <col min="33" max="33" width="4.68359375" customWidth="1"/>
     <col min="34" max="34" width="5" customWidth="1"/>
-    <col min="35" max="35" width="5.7109375" customWidth="1"/>
+    <col min="35" max="35" width="5.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="82" t="s">
+    <row r="1" spans="1:37" ht="15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="105" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
       <c r="K1" s="1"/>
-      <c r="L1" s="82" t="s">
+      <c r="L1" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="82"/>
-      <c r="R1" s="82"/>
-      <c r="S1" s="82"/>
-      <c r="T1" s="82"/>
-      <c r="U1" s="82"/>
+      <c r="M1" s="105"/>
+      <c r="N1" s="105"/>
+      <c r="O1" s="105"/>
+      <c r="P1" s="105"/>
+      <c r="Q1" s="105"/>
+      <c r="R1" s="105"/>
+      <c r="S1" s="105"/>
+      <c r="T1" s="105"/>
+      <c r="U1" s="105"/>
       <c r="V1" s="1"/>
-      <c r="W1" s="83" t="s">
+      <c r="W1" s="106" t="s">
         <v>106</v>
       </c>
-      <c r="X1" s="82"/>
-      <c r="Y1" s="82"/>
-      <c r="Z1" s="82"/>
-      <c r="AA1" s="82"/>
-      <c r="AB1" s="82"/>
-      <c r="AC1" s="82"/>
-      <c r="AD1" s="82"/>
-      <c r="AE1" s="82"/>
+      <c r="X1" s="105"/>
+      <c r="Y1" s="105"/>
+      <c r="Z1" s="105"/>
+      <c r="AA1" s="105"/>
+      <c r="AB1" s="105"/>
+      <c r="AC1" s="105"/>
+      <c r="AD1" s="105"/>
+      <c r="AE1" s="105"/>
     </row>
-    <row r="2" spans="1:37" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="K2" s="2"/>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:37" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" ht="12.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="52" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="52"/>
       <c r="C3" s="52"/>
-      <c r="D3" s="63" t="s">
+      <c r="D3" s="86" t="s">
         <v>107</v>
       </c>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64"/>
-      <c r="M3" s="64"/>
-      <c r="N3" s="64"/>
-      <c r="O3" s="64"/>
-      <c r="P3" s="65"/>
-      <c r="Q3" s="63" t="s">
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
+      <c r="O3" s="87"/>
+      <c r="P3" s="88"/>
+      <c r="Q3" s="86" t="s">
         <v>108</v>
       </c>
-      <c r="R3" s="64"/>
-      <c r="S3" s="64"/>
-      <c r="T3" s="64"/>
-      <c r="U3" s="64"/>
-      <c r="V3" s="64"/>
-      <c r="W3" s="64"/>
-      <c r="X3" s="64"/>
-      <c r="Y3" s="64"/>
-      <c r="Z3" s="64"/>
-      <c r="AA3" s="64"/>
-      <c r="AB3" s="64"/>
-      <c r="AC3" s="64"/>
-      <c r="AD3" s="64"/>
-      <c r="AE3" s="64"/>
-      <c r="AF3" s="65"/>
-      <c r="AG3" s="63" t="s">
+      <c r="R3" s="87"/>
+      <c r="S3" s="87"/>
+      <c r="T3" s="87"/>
+      <c r="U3" s="87"/>
+      <c r="V3" s="87"/>
+      <c r="W3" s="87"/>
+      <c r="X3" s="87"/>
+      <c r="Y3" s="87"/>
+      <c r="Z3" s="87"/>
+      <c r="AA3" s="87"/>
+      <c r="AB3" s="87"/>
+      <c r="AC3" s="87"/>
+      <c r="AD3" s="87"/>
+      <c r="AE3" s="87"/>
+      <c r="AF3" s="88"/>
+      <c r="AG3" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="AH3" s="64"/>
-      <c r="AI3" s="65"/>
+      <c r="AH3" s="87"/>
+      <c r="AI3" s="88"/>
     </row>
-    <row r="4" spans="1:37" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:37" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A4" s="52"/>
       <c r="B4" s="52"/>
       <c r="C4" s="52"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="67"/>
-      <c r="L4" s="67"/>
-      <c r="M4" s="67"/>
-      <c r="N4" s="67"/>
-      <c r="O4" s="67"/>
-      <c r="P4" s="68"/>
-      <c r="Q4" s="66"/>
-      <c r="R4" s="67"/>
-      <c r="S4" s="67"/>
-      <c r="T4" s="67"/>
-      <c r="U4" s="67"/>
-      <c r="V4" s="67"/>
-      <c r="W4" s="67"/>
-      <c r="X4" s="67"/>
-      <c r="Y4" s="67"/>
-      <c r="Z4" s="67"/>
-      <c r="AA4" s="67"/>
-      <c r="AB4" s="67"/>
-      <c r="AC4" s="67"/>
-      <c r="AD4" s="67"/>
-      <c r="AE4" s="67"/>
-      <c r="AF4" s="68"/>
-      <c r="AG4" s="66"/>
-      <c r="AH4" s="67"/>
-      <c r="AI4" s="68"/>
+      <c r="D4" s="89"/>
+      <c r="E4" s="90"/>
+      <c r="F4" s="90"/>
+      <c r="G4" s="90"/>
+      <c r="H4" s="90"/>
+      <c r="I4" s="90"/>
+      <c r="J4" s="90"/>
+      <c r="K4" s="90"/>
+      <c r="L4" s="90"/>
+      <c r="M4" s="90"/>
+      <c r="N4" s="90"/>
+      <c r="O4" s="90"/>
+      <c r="P4" s="91"/>
+      <c r="Q4" s="89"/>
+      <c r="R4" s="90"/>
+      <c r="S4" s="90"/>
+      <c r="T4" s="90"/>
+      <c r="U4" s="90"/>
+      <c r="V4" s="90"/>
+      <c r="W4" s="90"/>
+      <c r="X4" s="90"/>
+      <c r="Y4" s="90"/>
+      <c r="Z4" s="90"/>
+      <c r="AA4" s="90"/>
+      <c r="AB4" s="90"/>
+      <c r="AC4" s="90"/>
+      <c r="AD4" s="90"/>
+      <c r="AE4" s="90"/>
+      <c r="AF4" s="91"/>
+      <c r="AG4" s="89"/>
+      <c r="AH4" s="90"/>
+      <c r="AI4" s="91"/>
     </row>
-    <row r="5" spans="1:37" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:37" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A5" s="52"/>
       <c r="B5" s="52"/>
       <c r="C5" s="52"/>
-      <c r="D5" s="104"/>
-      <c r="E5" s="104"/>
-      <c r="F5" s="104"/>
-      <c r="G5" s="104"/>
-      <c r="H5" s="104"/>
-      <c r="I5" s="104"/>
-      <c r="J5" s="104"/>
-      <c r="K5" s="104"/>
-      <c r="L5" s="104"/>
-      <c r="M5" s="104"/>
-      <c r="N5" s="104"/>
-      <c r="O5" s="104"/>
-      <c r="P5" s="104"/>
-      <c r="Q5" s="104"/>
-      <c r="R5" s="104"/>
-      <c r="S5" s="104"/>
-      <c r="T5" s="104"/>
-      <c r="U5" s="104"/>
-      <c r="V5" s="104"/>
-      <c r="W5" s="104"/>
-      <c r="X5" s="104"/>
-      <c r="Y5" s="104"/>
-      <c r="Z5" s="104"/>
-      <c r="AA5" s="104"/>
-      <c r="AB5" s="104"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="59"/>
+      <c r="N5" s="59"/>
+      <c r="O5" s="59"/>
+      <c r="P5" s="59"/>
+      <c r="Q5" s="59"/>
+      <c r="R5" s="59"/>
+      <c r="S5" s="59"/>
+      <c r="T5" s="59"/>
+      <c r="U5" s="59"/>
+      <c r="V5" s="59"/>
+      <c r="W5" s="59"/>
+      <c r="X5" s="59"/>
+      <c r="Y5" s="59"/>
+      <c r="Z5" s="59"/>
+      <c r="AA5" s="59"/>
+      <c r="AB5" s="59"/>
       <c r="AC5" s="57"/>
       <c r="AD5" s="57"/>
       <c r="AE5" s="57"/>
@@ -2086,114 +2086,114 @@
       <c r="AH5" s="57"/>
       <c r="AI5" s="58"/>
     </row>
-    <row r="6" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="79" t="s">
+    <row r="6" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A6" s="133" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="80"/>
-      <c r="C6" s="80"/>
-      <c r="D6" s="80"/>
-      <c r="E6" s="80"/>
-      <c r="F6" s="80"/>
-      <c r="G6" s="80"/>
-      <c r="H6" s="81"/>
-      <c r="I6" s="84" t="s">
+      <c r="B6" s="134"/>
+      <c r="C6" s="134"/>
+      <c r="D6" s="134"/>
+      <c r="E6" s="134"/>
+      <c r="F6" s="134"/>
+      <c r="G6" s="134"/>
+      <c r="H6" s="135"/>
+      <c r="I6" s="107" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="98"/>
-      <c r="K6" s="84" t="s">
+      <c r="J6" s="125"/>
+      <c r="K6" s="107" t="s">
         <v>4</v>
       </c>
-      <c r="L6" s="85"/>
-      <c r="M6" s="100" t="s">
+      <c r="L6" s="108"/>
+      <c r="M6" s="127" t="s">
         <v>5</v>
       </c>
-      <c r="N6" s="101"/>
-      <c r="O6" s="84" t="s">
+      <c r="N6" s="128"/>
+      <c r="O6" s="107" t="s">
         <v>22</v>
       </c>
-      <c r="P6" s="85"/>
-      <c r="Q6" s="88" t="s">
+      <c r="P6" s="108"/>
+      <c r="Q6" s="113" t="s">
         <v>23</v>
       </c>
-      <c r="R6" s="89"/>
-      <c r="S6" s="89"/>
-      <c r="T6" s="89"/>
-      <c r="U6" s="75" t="s">
+      <c r="R6" s="114"/>
+      <c r="S6" s="114"/>
+      <c r="T6" s="114"/>
+      <c r="U6" s="111" t="s">
         <v>100</v>
       </c>
-      <c r="V6" s="76"/>
-      <c r="W6" s="75" t="s">
+      <c r="V6" s="112"/>
+      <c r="W6" s="111" t="s">
         <v>13</v>
       </c>
-      <c r="X6" s="76"/>
-      <c r="Y6" s="59" t="s">
+      <c r="X6" s="112"/>
+      <c r="Y6" s="101" t="s">
         <v>29</v>
       </c>
-      <c r="Z6" s="60"/>
-      <c r="AA6" s="59" t="s">
+      <c r="Z6" s="102"/>
+      <c r="AA6" s="101" t="s">
         <v>32</v>
       </c>
-      <c r="AB6" s="60"/>
-      <c r="AC6" s="71" t="s">
+      <c r="AB6" s="102"/>
+      <c r="AC6" s="95" t="s">
         <v>92</v>
       </c>
-      <c r="AD6" s="72"/>
-      <c r="AE6" s="72"/>
-      <c r="AF6" s="72"/>
-      <c r="AG6" s="72"/>
-      <c r="AH6" s="72"/>
-      <c r="AI6" s="73"/>
+      <c r="AD6" s="96"/>
+      <c r="AE6" s="96"/>
+      <c r="AF6" s="96"/>
+      <c r="AG6" s="96"/>
+      <c r="AH6" s="96"/>
+      <c r="AI6" s="97"/>
       <c r="AJ6" s="8"/>
       <c r="AK6" s="8"/>
     </row>
-    <row r="7" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="94" t="s">
+    <row r="7" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A7" s="121" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="95"/>
-      <c r="C7" s="92" t="s">
+      <c r="B7" s="122"/>
+      <c r="C7" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="93"/>
-      <c r="E7" s="94" t="s">
+      <c r="D7" s="120"/>
+      <c r="E7" s="121" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="95"/>
-      <c r="G7" s="96" t="s">
+      <c r="F7" s="122"/>
+      <c r="G7" s="123" t="s">
         <v>98</v>
       </c>
-      <c r="H7" s="97"/>
-      <c r="I7" s="86"/>
-      <c r="J7" s="99"/>
-      <c r="K7" s="86"/>
-      <c r="L7" s="87"/>
-      <c r="M7" s="102" t="s">
+      <c r="H7" s="124"/>
+      <c r="I7" s="109"/>
+      <c r="J7" s="126"/>
+      <c r="K7" s="109"/>
+      <c r="L7" s="110"/>
+      <c r="M7" s="129" t="s">
         <v>57</v>
       </c>
-      <c r="N7" s="103"/>
-      <c r="O7" s="86"/>
-      <c r="P7" s="87"/>
-      <c r="Q7" s="90"/>
-      <c r="R7" s="91"/>
-      <c r="S7" s="91"/>
-      <c r="T7" s="91"/>
-      <c r="U7" s="77" t="s">
+      <c r="N7" s="130"/>
+      <c r="O7" s="109"/>
+      <c r="P7" s="110"/>
+      <c r="Q7" s="115"/>
+      <c r="R7" s="116"/>
+      <c r="S7" s="116"/>
+      <c r="T7" s="116"/>
+      <c r="U7" s="117" t="s">
         <v>71</v>
       </c>
-      <c r="V7" s="78"/>
-      <c r="W7" s="77" t="s">
+      <c r="V7" s="118"/>
+      <c r="W7" s="117" t="s">
         <v>14</v>
       </c>
-      <c r="X7" s="78"/>
-      <c r="Y7" s="61" t="s">
+      <c r="X7" s="118"/>
+      <c r="Y7" s="103" t="s">
         <v>30</v>
       </c>
-      <c r="Z7" s="62"/>
-      <c r="AA7" s="61" t="s">
+      <c r="Z7" s="104"/>
+      <c r="AA7" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="AB7" s="62"/>
+      <c r="AB7" s="104"/>
       <c r="AC7" s="44"/>
       <c r="AD7" s="37" t="s">
         <v>42</v>
@@ -2216,7 +2216,7 @@
       <c r="AJ7" s="8"/>
       <c r="AK7" s="8"/>
     </row>
-    <row r="8" spans="1:37" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="56">
         <v>1</v>
       </c>
@@ -2285,7 +2285,7 @@
       <c r="AJ8" s="8"/>
       <c r="AK8" s="8"/>
     </row>
-    <row r="9" spans="1:37" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="31">
         <v>2</v>
       </c>
@@ -2354,7 +2354,7 @@
       <c r="AJ9" s="8"/>
       <c r="AK9" s="8"/>
     </row>
-    <row r="10" spans="1:37" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="31">
         <v>3</v>
       </c>
@@ -2423,7 +2423,7 @@
       <c r="AJ10" s="8"/>
       <c r="AK10" s="8"/>
     </row>
-    <row r="11" spans="1:37" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="31">
         <v>4</v>
       </c>
@@ -2490,7 +2490,7 @@
       <c r="AJ11" s="8"/>
       <c r="AK11" s="8"/>
     </row>
-    <row r="12" spans="1:37" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="31">
         <v>5</v>
       </c>
@@ -2557,7 +2557,7 @@
       <c r="AJ12" s="8"/>
       <c r="AK12" s="8"/>
     </row>
-    <row r="13" spans="1:37" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="31">
         <v>6</v>
       </c>
@@ -2602,7 +2602,9 @@
       <c r="V13" s="5"/>
       <c r="W13" s="5"/>
       <c r="X13" s="5"/>
-      <c r="Y13" s="5"/>
+      <c r="Y13" s="5">
+        <v>6</v>
+      </c>
       <c r="Z13" s="5"/>
       <c r="AA13" s="5"/>
       <c r="AB13" s="5"/>
@@ -2618,7 +2620,7 @@
       <c r="AJ13" s="8"/>
       <c r="AK13" s="8"/>
     </row>
-    <row r="14" spans="1:37" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="31">
         <v>7</v>
       </c>
@@ -2677,7 +2679,7 @@
       <c r="AJ14" s="8"/>
       <c r="AK14" s="8"/>
     </row>
-    <row r="15" spans="1:37" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="31">
         <v>8</v>
       </c>
@@ -2738,7 +2740,7 @@
       <c r="AJ15" s="8"/>
       <c r="AK15" s="8"/>
     </row>
-    <row r="16" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A16" s="31">
         <v>9</v>
       </c>
@@ -2799,7 +2801,7 @@
       <c r="AJ16" s="8"/>
       <c r="AK16" s="8"/>
     </row>
-    <row r="17" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A17" s="31">
         <v>10</v>
       </c>
@@ -2836,22 +2838,22 @@
       <c r="R17" s="5"/>
       <c r="S17" s="5"/>
       <c r="T17" s="6"/>
-      <c r="U17" s="69" t="s">
+      <c r="U17" s="82" t="s">
         <v>34</v>
       </c>
-      <c r="V17" s="74"/>
-      <c r="W17" s="69" t="s">
+      <c r="V17" s="83"/>
+      <c r="W17" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="X17" s="74"/>
-      <c r="Y17" s="69" t="s">
+      <c r="X17" s="83"/>
+      <c r="Y17" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="Z17" s="74"/>
-      <c r="AA17" s="69" t="s">
+      <c r="Z17" s="83"/>
+      <c r="AA17" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="AB17" s="74"/>
+      <c r="AB17" s="83"/>
       <c r="AC17" s="4" t="s">
         <v>146</v>
       </c>
@@ -2864,7 +2866,7 @@
       <c r="AJ17" s="8"/>
       <c r="AK17" s="8"/>
     </row>
-    <row r="18" spans="1:37" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="31">
         <v>11</v>
       </c>
@@ -2929,7 +2931,7 @@
       <c r="AJ18" s="8"/>
       <c r="AK18" s="8"/>
     </row>
-    <row r="19" spans="1:37" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="32">
         <v>12</v>
       </c>
@@ -2996,7 +2998,7 @@
       <c r="AJ19" s="8"/>
       <c r="AK19" s="8"/>
     </row>
-    <row r="20" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A20" s="32"/>
       <c r="B20" s="4"/>
       <c r="C20" s="3">
@@ -3061,7 +3063,7 @@
       <c r="AJ20" s="8"/>
       <c r="AK20" s="8"/>
     </row>
-    <row r="21" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A21" s="32"/>
       <c r="B21" s="4"/>
       <c r="C21" s="3">
@@ -3116,19 +3118,19 @@
         <v>4</v>
       </c>
       <c r="AB21" s="24"/>
-      <c r="AC21" s="115" t="s">
+      <c r="AC21" s="92" t="s">
         <v>64</v>
       </c>
-      <c r="AD21" s="116"/>
-      <c r="AE21" s="116"/>
-      <c r="AF21" s="116"/>
-      <c r="AG21" s="116"/>
-      <c r="AH21" s="116"/>
-      <c r="AI21" s="117"/>
+      <c r="AD21" s="93"/>
+      <c r="AE21" s="93"/>
+      <c r="AF21" s="93"/>
+      <c r="AG21" s="93"/>
+      <c r="AH21" s="93"/>
+      <c r="AI21" s="94"/>
       <c r="AJ21" s="8"/>
       <c r="AK21" s="8"/>
     </row>
-    <row r="22" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A22" s="51"/>
       <c r="B22" s="48"/>
       <c r="C22" s="3">
@@ -3151,7 +3153,7 @@
         <v>15</v>
       </c>
       <c r="L22" s="4"/>
-      <c r="M22" s="134"/>
+      <c r="M22" s="78"/>
       <c r="N22" s="26"/>
       <c r="O22" s="4">
         <v>15</v>
@@ -3187,13 +3189,13 @@
       <c r="AH22" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="AI22" s="139" t="s">
+      <c r="AI22" s="81" t="s">
         <v>91</v>
       </c>
       <c r="AJ22" s="8"/>
       <c r="AK22" s="8"/>
     </row>
-    <row r="23" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A23" s="51"/>
       <c r="B23" s="48"/>
       <c r="C23" s="3">
@@ -3214,10 +3216,10 @@
         <v>16</v>
       </c>
       <c r="L23" s="28"/>
-      <c r="M23" s="94" t="s">
+      <c r="M23" s="121" t="s">
         <v>58</v>
       </c>
-      <c r="N23" s="95"/>
+      <c r="N23" s="122"/>
       <c r="O23" s="41">
         <v>16</v>
       </c>
@@ -3246,7 +3248,7 @@
       <c r="AJ23" s="8"/>
       <c r="AK23" s="8"/>
     </row>
-    <row r="24" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A24" s="32"/>
       <c r="B24" s="4"/>
       <c r="C24" s="3">
@@ -3305,7 +3307,7 @@
       <c r="AJ24" s="8"/>
       <c r="AK24" s="8"/>
     </row>
-    <row r="25" spans="1:37" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="32"/>
       <c r="B25" s="4"/>
       <c r="C25" s="3"/>
@@ -3324,7 +3326,7 @@
         <v>18</v>
       </c>
       <c r="L25" s="4"/>
-      <c r="M25" s="122">
+      <c r="M25" s="72">
         <v>16</v>
       </c>
       <c r="N25" s="9"/>
@@ -3340,18 +3342,18 @@
         <v>166</v>
       </c>
       <c r="T25" s="6"/>
-      <c r="U25" s="59" t="s">
+      <c r="U25" s="101" t="s">
         <v>101</v>
       </c>
-      <c r="V25" s="60"/>
-      <c r="W25" s="59" t="s">
+      <c r="V25" s="102"/>
+      <c r="W25" s="101" t="s">
         <v>102</v>
       </c>
-      <c r="X25" s="60"/>
-      <c r="Y25" s="59" t="s">
+      <c r="X25" s="102"/>
+      <c r="Y25" s="101" t="s">
         <v>49</v>
       </c>
-      <c r="Z25" s="60"/>
+      <c r="Z25" s="102"/>
       <c r="AA25" s="36"/>
       <c r="AB25" s="17"/>
       <c r="AC25" s="5" t="s">
@@ -3366,7 +3368,7 @@
       <c r="AJ25" s="8"/>
       <c r="AK25" s="8"/>
     </row>
-    <row r="26" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A26" s="45"/>
       <c r="B26" s="4"/>
       <c r="C26" s="3"/>
@@ -3397,18 +3399,18 @@
       <c r="R26" s="5"/>
       <c r="S26" s="5"/>
       <c r="T26" s="6"/>
-      <c r="U26" s="61" t="s">
+      <c r="U26" s="103" t="s">
         <v>33</v>
       </c>
-      <c r="V26" s="62"/>
-      <c r="W26" s="61" t="s">
+      <c r="V26" s="104"/>
+      <c r="W26" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="X26" s="62"/>
-      <c r="Y26" s="61" t="s">
+      <c r="X26" s="104"/>
+      <c r="Y26" s="103" t="s">
         <v>74</v>
       </c>
-      <c r="Z26" s="62"/>
+      <c r="Z26" s="104"/>
       <c r="AA26" s="36"/>
       <c r="AB26" s="17"/>
       <c r="AC26" s="5" t="s">
@@ -3423,7 +3425,7 @@
       <c r="AJ26" s="8"/>
       <c r="AK26" s="8"/>
     </row>
-    <row r="27" spans="1:37" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="32"/>
       <c r="B27" s="4"/>
       <c r="C27" s="3"/>
@@ -3478,10 +3480,10 @@
       <c r="AJ27" s="8"/>
       <c r="AK27" s="8"/>
     </row>
-    <row r="28" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A28" s="32"/>
       <c r="B28" s="4"/>
-      <c r="C28" s="123"/>
+      <c r="C28" s="73"/>
       <c r="D28" s="4"/>
       <c r="E28" s="3"/>
       <c r="F28" s="4"/>
@@ -3535,14 +3537,14 @@
       <c r="AJ28" s="8"/>
       <c r="AK28" s="8"/>
     </row>
-    <row r="29" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A29" s="47"/>
       <c r="B29" s="35"/>
-      <c r="C29" s="124"/>
-      <c r="D29" s="125"/>
+      <c r="C29" s="74"/>
+      <c r="D29" s="75"/>
       <c r="E29" s="3"/>
       <c r="F29" s="4"/>
-      <c r="G29" s="126"/>
+      <c r="G29" s="76"/>
       <c r="H29" s="4"/>
       <c r="I29" s="3"/>
       <c r="J29" s="4"/>
@@ -3580,26 +3582,26 @@
       <c r="Z29" s="17"/>
       <c r="AA29" s="5"/>
       <c r="AB29" s="24"/>
-      <c r="AC29" s="71" t="s">
+      <c r="AC29" s="95" t="s">
         <v>75</v>
       </c>
-      <c r="AD29" s="72"/>
-      <c r="AE29" s="72"/>
-      <c r="AF29" s="72"/>
-      <c r="AG29" s="72"/>
-      <c r="AH29" s="72"/>
-      <c r="AI29" s="73"/>
+      <c r="AD29" s="96"/>
+      <c r="AE29" s="96"/>
+      <c r="AF29" s="96"/>
+      <c r="AG29" s="96"/>
+      <c r="AH29" s="96"/>
+      <c r="AI29" s="97"/>
       <c r="AJ29" s="8"/>
       <c r="AK29" s="8"/>
     </row>
-    <row r="30" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A30" s="33"/>
       <c r="B30" s="26"/>
       <c r="C30" s="46"/>
       <c r="D30" s="46"/>
       <c r="E30" s="46"/>
       <c r="F30" s="46"/>
-      <c r="G30" s="105"/>
+      <c r="G30" s="60"/>
       <c r="H30" s="46"/>
       <c r="I30" s="35"/>
       <c r="J30" s="4"/>
@@ -3607,7 +3609,7 @@
         <v>23</v>
       </c>
       <c r="L30" s="4"/>
-      <c r="M30" s="134"/>
+      <c r="M30" s="78"/>
       <c r="N30" s="27"/>
       <c r="O30" s="4">
         <v>23</v>
@@ -3645,44 +3647,44 @@
         <v>39</v>
       </c>
       <c r="AH30" s="11"/>
-      <c r="AI30" s="139"/>
+      <c r="AI30" s="81"/>
       <c r="AJ30" s="8"/>
       <c r="AK30" s="8"/>
     </row>
-    <row r="31" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="115" t="s">
+    <row r="31" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A31" s="92" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="128"/>
-      <c r="C31" s="115" t="s">
+      <c r="B31" s="131"/>
+      <c r="C31" s="92" t="s">
         <v>99</v>
       </c>
-      <c r="D31" s="117"/>
-      <c r="E31" s="71" t="s">
+      <c r="D31" s="94"/>
+      <c r="E31" s="95" t="s">
         <v>11</v>
       </c>
-      <c r="F31" s="73"/>
-      <c r="G31" s="129" t="s">
+      <c r="F31" s="97"/>
+      <c r="G31" s="132" t="s">
         <v>147</v>
       </c>
-      <c r="H31" s="73"/>
+      <c r="H31" s="97"/>
       <c r="I31" s="43"/>
       <c r="J31" s="4"/>
       <c r="K31" s="3">
         <v>24</v>
       </c>
       <c r="L31" s="28"/>
-      <c r="M31" s="94" t="s">
+      <c r="M31" s="121" t="s">
         <v>59</v>
       </c>
-      <c r="N31" s="95"/>
+      <c r="N31" s="122"/>
       <c r="O31" s="41">
         <v>24</v>
       </c>
       <c r="P31" s="4"/>
       <c r="Q31" s="39"/>
       <c r="R31" s="17"/>
-      <c r="S31" s="120"/>
+      <c r="S31" s="70"/>
       <c r="T31" s="17"/>
       <c r="U31" s="17"/>
       <c r="V31" s="17"/>
@@ -3704,7 +3706,7 @@
       <c r="AJ31" s="8"/>
       <c r="AK31" s="8"/>
     </row>
-    <row r="32" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A32" s="34"/>
       <c r="B32" s="13"/>
       <c r="C32" s="11">
@@ -3759,7 +3761,7 @@
       <c r="AJ32" s="8"/>
       <c r="AK32" s="8"/>
     </row>
-    <row r="33" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A33" s="32">
         <v>8</v>
       </c>
@@ -3796,20 +3798,20 @@
       <c r="R33" s="17"/>
       <c r="S33" s="4"/>
       <c r="T33" s="6"/>
-      <c r="U33" s="69" t="s">
+      <c r="U33" s="82" t="s">
         <v>31</v>
       </c>
-      <c r="V33" s="70"/>
-      <c r="W33" s="70"/>
-      <c r="X33" s="74"/>
-      <c r="Y33" s="69" t="s">
+      <c r="V33" s="100"/>
+      <c r="W33" s="100"/>
+      <c r="X33" s="83"/>
+      <c r="Y33" s="82" t="s">
         <v>104</v>
       </c>
-      <c r="Z33" s="74"/>
-      <c r="AA33" s="69" t="s">
+      <c r="Z33" s="83"/>
+      <c r="AA33" s="82" t="s">
         <v>103</v>
       </c>
-      <c r="AB33" s="74"/>
+      <c r="AB33" s="83"/>
       <c r="AC33" s="16" t="s">
         <v>78</v>
       </c>
@@ -3822,7 +3824,7 @@
       <c r="AJ33" s="8"/>
       <c r="AK33" s="8"/>
     </row>
-    <row r="34" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A34" s="32">
         <v>10</v>
       </c>
@@ -3859,7 +3861,7 @@
         <v>1</v>
       </c>
       <c r="V34" s="11"/>
-      <c r="W34" s="138" t="s">
+      <c r="W34" s="80" t="s">
         <v>47</v>
       </c>
       <c r="X34" s="11"/>
@@ -3881,7 +3883,7 @@
       <c r="AJ34" s="8"/>
       <c r="AK34" s="8"/>
     </row>
-    <row r="35" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A35" s="32">
         <v>12</v>
       </c>
@@ -3918,7 +3920,7 @@
         <v>2</v>
       </c>
       <c r="V35" s="5"/>
-      <c r="W35" s="138" t="s">
+      <c r="W35" s="80" t="s">
         <v>48</v>
       </c>
       <c r="X35" s="5"/>
@@ -3930,19 +3932,19 @@
         <v>2</v>
       </c>
       <c r="AB35" s="50"/>
-      <c r="AC35" s="115" t="s">
+      <c r="AC35" s="92" t="s">
         <v>93</v>
       </c>
-      <c r="AD35" s="116"/>
-      <c r="AE35" s="116"/>
-      <c r="AF35" s="116"/>
-      <c r="AG35" s="116"/>
-      <c r="AH35" s="116"/>
-      <c r="AI35" s="117"/>
+      <c r="AD35" s="93"/>
+      <c r="AE35" s="93"/>
+      <c r="AF35" s="93"/>
+      <c r="AG35" s="93"/>
+      <c r="AH35" s="93"/>
+      <c r="AI35" s="94"/>
       <c r="AJ35" s="8"/>
       <c r="AK35" s="8"/>
     </row>
-    <row r="36" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A36" s="32">
         <v>13</v>
       </c>
@@ -3997,11 +3999,11 @@
         <v>40</v>
       </c>
       <c r="AH36" s="11"/>
-      <c r="AI36" s="139"/>
+      <c r="AI36" s="81"/>
       <c r="AJ36" s="8"/>
       <c r="AK36" s="8"/>
     </row>
-    <row r="37" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A37" s="32"/>
       <c r="B37" s="4"/>
       <c r="C37" s="5">
@@ -4016,10 +4018,10 @@
         <v>153</v>
       </c>
       <c r="H37" s="28"/>
-      <c r="I37" s="130" t="s">
+      <c r="I37" s="136" t="s">
         <v>18</v>
       </c>
-      <c r="J37" s="131"/>
+      <c r="J37" s="137"/>
       <c r="K37" s="41"/>
       <c r="L37" s="4"/>
       <c r="M37" s="10">
@@ -4030,13 +4032,13 @@
         <v>30</v>
       </c>
       <c r="P37" s="28"/>
-      <c r="Q37" s="69" t="s">
+      <c r="Q37" s="82" t="s">
         <v>90</v>
       </c>
-      <c r="R37" s="70"/>
-      <c r="S37" s="70"/>
-      <c r="T37" s="74"/>
-      <c r="U37" s="106"/>
+      <c r="R37" s="100"/>
+      <c r="S37" s="100"/>
+      <c r="T37" s="83"/>
+      <c r="U37" s="61"/>
       <c r="V37" s="14"/>
       <c r="W37" s="5"/>
       <c r="X37" s="5"/>
@@ -4056,7 +4058,7 @@
       <c r="AJ37" s="8"/>
       <c r="AK37" s="8"/>
     </row>
-    <row r="38" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A38" s="32"/>
       <c r="B38" s="4"/>
       <c r="C38" s="5">
@@ -4071,8 +4073,8 @@
         <v>158</v>
       </c>
       <c r="H38" s="6"/>
-      <c r="I38" s="132"/>
-      <c r="J38" s="133"/>
+      <c r="I38" s="138"/>
+      <c r="J38" s="139"/>
       <c r="K38" s="41"/>
       <c r="L38" s="4"/>
       <c r="M38" s="10"/>
@@ -4089,22 +4091,22 @@
         <v>9</v>
       </c>
       <c r="T38" s="7"/>
-      <c r="U38" s="118" t="s">
+      <c r="U38" s="98" t="s">
         <v>63</v>
       </c>
-      <c r="V38" s="119"/>
-      <c r="W38" s="118" t="s">
+      <c r="V38" s="99"/>
+      <c r="W38" s="98" t="s">
         <v>61</v>
       </c>
-      <c r="X38" s="119"/>
-      <c r="Y38" s="118" t="s">
+      <c r="X38" s="99"/>
+      <c r="Y38" s="98" t="s">
         <v>105</v>
       </c>
-      <c r="Z38" s="119"/>
-      <c r="AA38" s="118" t="s">
+      <c r="Z38" s="99"/>
+      <c r="AA38" s="98" t="s">
         <v>62</v>
       </c>
-      <c r="AB38" s="119"/>
+      <c r="AB38" s="99"/>
       <c r="AC38" s="16" t="s">
         <v>96</v>
       </c>
@@ -4117,7 +4119,7 @@
       <c r="AJ38" s="8"/>
       <c r="AK38" s="8"/>
     </row>
-    <row r="39" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A39" s="32"/>
       <c r="B39" s="4"/>
       <c r="C39" s="5">
@@ -4152,22 +4154,22 @@
         <v>46</v>
       </c>
       <c r="T39" s="24"/>
-      <c r="U39" s="136" t="s">
+      <c r="U39" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="V39" s="137"/>
-      <c r="W39" s="136" t="s">
+      <c r="V39" s="85"/>
+      <c r="W39" s="84" t="s">
         <v>36</v>
       </c>
-      <c r="X39" s="137"/>
-      <c r="Y39" s="136" t="s">
+      <c r="X39" s="85"/>
+      <c r="Y39" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="Z39" s="137"/>
-      <c r="AA39" s="136" t="s">
+      <c r="Z39" s="85"/>
+      <c r="AA39" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="AB39" s="137"/>
+      <c r="AB39" s="85"/>
       <c r="AC39" s="16" t="s">
         <v>97</v>
       </c>
@@ -4180,7 +4182,7 @@
       <c r="AJ39" s="8"/>
       <c r="AK39" s="8"/>
     </row>
-    <row r="40" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:37" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="15"/>
       <c r="B40" s="5"/>
       <c r="C40" s="35"/>
@@ -4207,7 +4209,7 @@
         <v>51</v>
       </c>
       <c r="T40" s="35"/>
-      <c r="U40" s="135" t="s">
+      <c r="U40" s="79" t="s">
         <v>44</v>
       </c>
       <c r="V40" s="11"/>
@@ -4235,7 +4237,7 @@
       <c r="AJ40" s="8"/>
       <c r="AK40" s="8"/>
     </row>
-    <row r="41" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:37" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="15"/>
       <c r="B41" s="5"/>
       <c r="C41" s="35"/>
@@ -4244,7 +4246,7 @@
       <c r="F41" s="35"/>
       <c r="G41" s="48"/>
       <c r="H41" s="35"/>
-      <c r="I41" s="127">
+      <c r="I41" s="77">
         <v>2</v>
       </c>
       <c r="J41" s="5"/>
@@ -4263,8 +4265,8 @@
       <c r="S41" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="T41" s="120"/>
-      <c r="U41" s="121" t="s">
+      <c r="T41" s="70"/>
+      <c r="U41" s="71" t="s">
         <v>45</v>
       </c>
       <c r="V41" s="17"/>
@@ -4292,23 +4294,23 @@
       <c r="AJ41" s="8"/>
       <c r="AK41" s="8"/>
     </row>
-    <row r="42" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="109"/>
-      <c r="B42" s="107"/>
-      <c r="C42" s="107"/>
-      <c r="D42" s="107"/>
-      <c r="E42" s="107"/>
-      <c r="F42" s="107"/>
-      <c r="G42" s="108"/>
-      <c r="H42" s="107"/>
-      <c r="I42" s="107"/>
-      <c r="J42" s="107"/>
-      <c r="K42" s="107"/>
-      <c r="L42" s="107"/>
-      <c r="M42" s="107"/>
-      <c r="N42" s="107"/>
-      <c r="O42" s="107"/>
-      <c r="P42" s="107"/>
+    <row r="42" spans="1:37" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="64"/>
+      <c r="B42" s="62"/>
+      <c r="C42" s="62"/>
+      <c r="D42" s="62"/>
+      <c r="E42" s="62"/>
+      <c r="F42" s="62"/>
+      <c r="G42" s="63"/>
+      <c r="H42" s="62"/>
+      <c r="I42" s="62"/>
+      <c r="J42" s="62"/>
+      <c r="K42" s="62"/>
+      <c r="L42" s="62"/>
+      <c r="M42" s="62"/>
+      <c r="N42" s="62"/>
+      <c r="O42" s="62"/>
+      <c r="P42" s="62"/>
       <c r="Q42" s="4">
         <v>5</v>
       </c>
@@ -4316,7 +4318,7 @@
       <c r="S42" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="T42" s="120"/>
+      <c r="T42" s="70"/>
       <c r="U42" s="29"/>
       <c r="V42" s="17"/>
       <c r="W42" s="5">
@@ -4329,74 +4331,75 @@
         <v>3</v>
       </c>
       <c r="AB42" s="17"/>
-      <c r="AC42" s="107"/>
-      <c r="AD42" s="107"/>
-      <c r="AE42" s="107"/>
-      <c r="AF42" s="107"/>
-      <c r="AG42" s="107"/>
-      <c r="AH42" s="107"/>
-      <c r="AI42" s="110"/>
+      <c r="AC42" s="62"/>
+      <c r="AD42" s="62"/>
+      <c r="AE42" s="62"/>
+      <c r="AF42" s="62"/>
+      <c r="AG42" s="62"/>
+      <c r="AH42" s="62"/>
+      <c r="AI42" s="65"/>
     </row>
-    <row r="43" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="111"/>
-      <c r="B43" s="112"/>
-      <c r="C43" s="112"/>
-      <c r="D43" s="112"/>
-      <c r="E43" s="112"/>
-      <c r="F43" s="112"/>
-      <c r="G43" s="113"/>
-      <c r="H43" s="112"/>
-      <c r="I43" s="112"/>
-      <c r="J43" s="112"/>
-      <c r="K43" s="112"/>
-      <c r="L43" s="112"/>
-      <c r="M43" s="112"/>
-      <c r="N43" s="112"/>
-      <c r="O43" s="112" t="s">
+    <row r="43" spans="1:37" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A43" s="66"/>
+      <c r="B43" s="67"/>
+      <c r="C43" s="67"/>
+      <c r="D43" s="67"/>
+      <c r="E43" s="67"/>
+      <c r="F43" s="67"/>
+      <c r="G43" s="68"/>
+      <c r="H43" s="67"/>
+      <c r="I43" s="67"/>
+      <c r="J43" s="67"/>
+      <c r="K43" s="67"/>
+      <c r="L43" s="67"/>
+      <c r="M43" s="67"/>
+      <c r="N43" s="67"/>
+      <c r="O43" s="67" t="s">
         <v>160</v>
       </c>
-      <c r="P43" s="112"/>
-      <c r="Q43" s="112"/>
-      <c r="R43" s="112"/>
-      <c r="S43" s="112"/>
-      <c r="T43" s="112"/>
-      <c r="U43" s="112"/>
-      <c r="V43" s="112"/>
-      <c r="W43" s="112"/>
-      <c r="X43" s="112"/>
-      <c r="Y43" s="112"/>
-      <c r="Z43" s="112"/>
-      <c r="AA43" s="112"/>
-      <c r="AB43" s="112"/>
-      <c r="AC43" s="112"/>
-      <c r="AD43" s="112"/>
-      <c r="AE43" s="112"/>
-      <c r="AF43" s="112"/>
-      <c r="AG43" s="112"/>
-      <c r="AH43" s="112"/>
-      <c r="AI43" s="114"/>
+      <c r="P43" s="67"/>
+      <c r="Q43" s="67"/>
+      <c r="R43" s="67"/>
+      <c r="S43" s="67"/>
+      <c r="T43" s="67"/>
+      <c r="U43" s="67"/>
+      <c r="V43" s="67"/>
+      <c r="W43" s="67"/>
+      <c r="X43" s="67"/>
+      <c r="Y43" s="67"/>
+      <c r="Z43" s="67"/>
+      <c r="AA43" s="67"/>
+      <c r="AB43" s="67"/>
+      <c r="AC43" s="67"/>
+      <c r="AD43" s="67"/>
+      <c r="AE43" s="67"/>
+      <c r="AF43" s="67"/>
+      <c r="AG43" s="67"/>
+      <c r="AH43" s="67"/>
+      <c r="AI43" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="U17:V17"/>
-    <mergeCell ref="W17:X17"/>
-    <mergeCell ref="Y17:Z17"/>
-    <mergeCell ref="AA17:AB17"/>
-    <mergeCell ref="AA39:AB39"/>
-    <mergeCell ref="Q3:AF4"/>
-    <mergeCell ref="AG3:AI4"/>
-    <mergeCell ref="AC21:AI21"/>
-    <mergeCell ref="AC29:AI29"/>
-    <mergeCell ref="U38:V38"/>
-    <mergeCell ref="W38:X38"/>
-    <mergeCell ref="Y38:Z38"/>
-    <mergeCell ref="AA38:AB38"/>
-    <mergeCell ref="Q37:T37"/>
-    <mergeCell ref="U33:X33"/>
-    <mergeCell ref="Y33:Z33"/>
-    <mergeCell ref="AA33:AB33"/>
-    <mergeCell ref="U25:V25"/>
-    <mergeCell ref="U26:V26"/>
+    <mergeCell ref="D3:P4"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="Y6:Z6"/>
+    <mergeCell ref="Y7:Z7"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="AA7:AB7"/>
+    <mergeCell ref="U39:V39"/>
+    <mergeCell ref="W39:X39"/>
+    <mergeCell ref="Y39:Z39"/>
+    <mergeCell ref="I37:J38"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="W25:X25"/>
+    <mergeCell ref="W26:X26"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="L1:U1"/>
     <mergeCell ref="W1:AE1"/>
@@ -4413,29 +4416,28 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="M6:N6"/>
     <mergeCell ref="M7:N7"/>
+    <mergeCell ref="Q3:AF4"/>
+    <mergeCell ref="AG3:AI4"/>
+    <mergeCell ref="AC21:AI21"/>
+    <mergeCell ref="AC29:AI29"/>
+    <mergeCell ref="U38:V38"/>
+    <mergeCell ref="W38:X38"/>
+    <mergeCell ref="Y38:Z38"/>
+    <mergeCell ref="AA38:AB38"/>
+    <mergeCell ref="Q37:T37"/>
+    <mergeCell ref="U33:X33"/>
+    <mergeCell ref="Y33:Z33"/>
+    <mergeCell ref="AA33:AB33"/>
+    <mergeCell ref="U25:V25"/>
+    <mergeCell ref="U26:V26"/>
     <mergeCell ref="AC35:AI35"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="W25:X25"/>
-    <mergeCell ref="W26:X26"/>
     <mergeCell ref="Y25:Z25"/>
+    <mergeCell ref="U17:V17"/>
+    <mergeCell ref="W17:X17"/>
+    <mergeCell ref="Y17:Z17"/>
+    <mergeCell ref="AA17:AB17"/>
+    <mergeCell ref="AA39:AB39"/>
     <mergeCell ref="Y26:Z26"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="AA6:AB6"/>
-    <mergeCell ref="AA7:AB7"/>
-    <mergeCell ref="U39:V39"/>
-    <mergeCell ref="W39:X39"/>
-    <mergeCell ref="Y39:Z39"/>
-    <mergeCell ref="I37:J38"/>
-    <mergeCell ref="D3:P4"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="Y6:Z6"/>
-    <mergeCell ref="Y7:Z7"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="U7:V7"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
@@ -4456,7 +4458,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4468,7 +4470,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4480,7 +4482,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>